<commit_message>
Optimized for LTS operation
</commit_message>
<xml_diff>
--- a/academicpeak/code/database.xlsx
+++ b/academicpeak/code/database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xieho\PycharmProjects\hongzhe.site\academicpeak\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xieho\PycharmProjects\Academic-Peak\academicpeak\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1216A1A1-D995-48DB-8A2F-8F86C4F57950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7CCA22-A2A6-4653-8514-57E77293B987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2475" yWindow="4320" windowWidth="38700" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -227,10 +227,6 @@
     <t>https://www.nyu.edu/</t>
   </si>
   <si>
-    <t>Republic of China</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Yale University</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -313,6 +309,9 @@
   <si>
     <t>Stanford University.jpg</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>People's Republic of China</t>
   </si>
 </sst>
 </file>
@@ -649,18 +648,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="38.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="81.6640625" customWidth="1"/>
-    <col min="7" max="7" width="94.44140625" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="81.7109375" customWidth="1"/>
+    <col min="7" max="7" width="94.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -701,13 +700,13 @@
       </c>
       <c r="E2">
         <f ca="1">INT(RAND()*100000)</f>
-        <v>21728</v>
+        <v>34566</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -725,13 +724,13 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E22" ca="1" si="0">INT(RAND()*100000)</f>
-        <v>51870</v>
+        <v>11636</v>
       </c>
       <c r="F3" t="s">
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -749,13 +748,13 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>32412</v>
+        <v>73063</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -773,13 +772,13 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>80960</v>
+        <v>86862</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -787,7 +786,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
@@ -797,13 +796,13 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>22040</v>
+        <v>15846</v>
       </c>
       <c r="F6" t="s">
         <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -821,13 +820,13 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>34557</v>
+        <v>12419</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -838,20 +837,20 @@
         <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="D8">
         <v>88</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>70933</v>
+        <v>95165</v>
       </c>
       <c r="F8" t="s">
         <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -869,13 +868,13 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>60488</v>
+        <v>74991</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -893,13 +892,13 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>76752</v>
+        <v>48911</v>
       </c>
       <c r="F10" t="s">
         <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -907,7 +906,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
@@ -917,13 +916,13 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>55743</v>
+        <v>83361</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -931,7 +930,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
@@ -941,13 +940,13 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>21831</v>
+        <v>17278</v>
       </c>
       <c r="F12" t="s">
         <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -965,13 +964,13 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>98651</v>
+        <v>18654</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -989,13 +988,13 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>73821</v>
+        <v>68977</v>
       </c>
       <c r="F14" t="s">
         <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1003,23 +1002,23 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D15">
         <v>74</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>39311</v>
+        <v>10210</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1037,13 +1036,13 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>35191</v>
+        <v>79447</v>
       </c>
       <c r="F16" t="s">
         <v>36</v>
       </c>
       <c r="G16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1061,13 +1060,13 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>40298</v>
+        <v>76950</v>
       </c>
       <c r="F17" t="s">
         <v>37</v>
       </c>
       <c r="G17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1085,13 +1084,13 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>49803</v>
+        <v>12726</v>
       </c>
       <c r="F18" t="s">
         <v>39</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1109,13 +1108,13 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>85512</v>
+        <v>78173</v>
       </c>
       <c r="F19" t="s">
         <v>40</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1123,7 +1122,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
@@ -1133,13 +1132,13 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>56437</v>
+        <v>6330</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1147,23 +1146,23 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="D21">
         <v>62</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>94210</v>
+        <v>51702</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1181,13 +1180,13 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>94550</v>
+        <v>6007</v>
       </c>
       <c r="F22" t="s">
         <v>47</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1205,13 +1204,13 @@
       </c>
       <c r="E23">
         <f ca="1">INT(RAND()*100000)</f>
-        <v>40939</v>
+        <v>25437</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
       </c>
       <c r="G23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1229,13 +1228,13 @@
       </c>
       <c r="E24">
         <f ca="1">INT(RAND()*100000)</f>
-        <v>86029</v>
+        <v>62427</v>
       </c>
       <c r="F24" t="s">
         <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1253,13 +1252,13 @@
       </c>
       <c r="E25">
         <f ca="1">INT(RAND()*100000)</f>
-        <v>43918</v>
+        <v>66971</v>
       </c>
       <c r="F25" t="s">
         <v>31</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update some file and database
</commit_message>
<xml_diff>
--- a/academicpeak/code/database.xlsx
+++ b/academicpeak/code/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xieho\PycharmProjects\Academic-Peak\academicpeak\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3870FE1C-D960-4D86-86DA-F4A9C65CF658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B898124F-0D11-4282-B8AF-577B985A0296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5976" yWindow="0" windowWidth="17892" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
   <si>
     <t>Rank</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -295,10 +295,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>nyu-new-york-university-office.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>lse.jpg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -320,7 +316,19 @@
     <t>https://www.washington.edu/</t>
   </si>
   <si>
-    <t>University of Washington.png</t>
+    <t>University of Washington.jpg</t>
+  </si>
+  <si>
+    <t>NYU.jpg</t>
+  </si>
+  <si>
+    <t>UCSB.jpg</t>
+  </si>
+  <si>
+    <t>https://www.ucsb.edu/</t>
+  </si>
+  <si>
+    <t>UC: Santa Barbara</t>
   </si>
 </sst>
 </file>
@@ -655,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -698,8 +706,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>75</v>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -709,45 +717,45 @@
       </c>
       <c r="E2">
         <f ca="1">INT(RAND()*100000)</f>
-        <v>31306</v>
+        <v>95592</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+      <c r="B3" t="s">
+        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>98</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E22" ca="1" si="0">INT(RAND()*100000)</f>
-        <v>10502</v>
+        <v>53743</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>43</v>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
@@ -757,21 +765,21 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>71528</v>
+        <v>14879</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
+      <c r="B5" t="s">
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -781,13 +789,13 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>65994</v>
+        <v>7519</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -805,7 +813,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>54881</v>
+        <v>85572</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
@@ -829,7 +837,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>60269</v>
+        <v>17532</v>
       </c>
       <c r="F7" t="s">
         <v>38</v>
@@ -853,7 +861,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>79302</v>
+        <v>72130</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -866,24 +874,24 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>45</v>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>86</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>95671</v>
+        <v>67864</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -901,7 +909,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>54247</v>
+        <v>49967</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
@@ -925,13 +933,13 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>80626</v>
+        <v>79196</v>
       </c>
       <c r="F11" t="s">
         <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -949,13 +957,13 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>31675</v>
+        <v>60873</v>
       </c>
       <c r="F12" t="s">
         <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -963,23 +971,23 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <v>78</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>14189</v>
+        <v>12100</v>
       </c>
       <c r="F13" t="s">
         <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -987,23 +995,23 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>76</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>90728</v>
+        <v>25824</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1011,20 +1019,20 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15">
         <v>74</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>29022</v>
+        <v>5997</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" t="s">
         <v>64</v>
@@ -1035,20 +1043,20 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D16">
         <v>72</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>20013</v>
+        <v>14896</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s">
         <v>64</v>
@@ -1059,20 +1067,20 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="D17">
         <v>70</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>96416</v>
+        <v>81944</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
         <v>64</v>
@@ -1083,7 +1091,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -1093,10 +1101,10 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>95493</v>
+        <v>16632</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G18" t="s">
         <v>64</v>
@@ -1107,20 +1115,20 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D19">
         <v>66</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>5696</v>
+        <v>7294</v>
       </c>
       <c r="F19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G19" t="s">
         <v>64</v>
@@ -1131,20 +1139,20 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D20">
         <v>64</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>40472</v>
+        <v>78514</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G20" t="s">
         <v>64</v>
@@ -1155,7 +1163,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>15</v>
@@ -1165,10 +1173,10 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>14560</v>
+        <v>57671</v>
       </c>
       <c r="F21" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="G21" t="s">
         <v>64</v>
@@ -1179,20 +1187,20 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="D22">
         <v>60</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>29301</v>
+        <v>92366</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G22" t="s">
         <v>64</v>
@@ -1202,21 +1210,21 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>28</v>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="D23">
         <v>58</v>
       </c>
       <c r="E23">
         <f ca="1">INT(RAND()*100000)</f>
-        <v>87251</v>
+        <v>41902</v>
       </c>
       <c r="F23" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="G23" t="s">
         <v>64</v>
@@ -1226,21 +1234,21 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>16</v>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D24">
         <v>56</v>
       </c>
       <c r="E24">
         <f ca="1">INT(RAND()*100000)</f>
-        <v>39135</v>
+        <v>68396</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="G24" t="s">
         <v>64</v>
@@ -1250,24 +1258,24 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>29</v>
+      <c r="B25" t="s">
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="D25">
         <v>54</v>
       </c>
       <c r="E25">
         <f ca="1">INT(RAND()*100000)</f>
-        <v>65846</v>
+        <v>17825</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G25" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1275,7 +1283,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>22</v>
@@ -1285,35 +1293,60 @@
       </c>
       <c r="E26">
         <f ca="1">INT(RAND()*100000)</f>
-        <v>97223</v>
+        <v>20260</v>
       </c>
       <c r="F26" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27">
+        <v>50</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ref="E27" ca="1" si="1">INT(RAND()*100000)</f>
+        <v>31769</v>
+      </c>
+      <c r="F27" t="s">
         <v>31</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.topuniversities.com/universities/university-sheffield" xr:uid="{99983691-3A0A-4C3C-9F42-2E43E3A0B8A3}"/>
+    <hyperlink ref="B13" r:id="rId1" display="https://www.topuniversities.com/universities/university-sheffield" xr:uid="{99983691-3A0A-4C3C-9F42-2E43E3A0B8A3}"/>
     <hyperlink ref="B10" r:id="rId2" display="https://www.usnews.com/education/best-global-universities/harvard-university-166027" xr:uid="{7978A213-D431-46CF-8201-9BA0735B8A3F}"/>
     <hyperlink ref="B8" r:id="rId3" display="https://www.usnews.com/education/best-global-universities/university-of-california-berkeley-110635" xr:uid="{4D75220F-9B33-4F4D-8693-69911F9519C8}"/>
     <hyperlink ref="F8" r:id="rId4" xr:uid="{CDF58638-52C8-4B3B-AD1A-A2C6BA2650B4}"/>
     <hyperlink ref="F6" r:id="rId5" xr:uid="{D6A8DE96-784D-4552-9293-D51126E14D21}"/>
-    <hyperlink ref="F24" r:id="rId6" xr:uid="{D4ED1D55-E4AC-4C6B-85A0-E974BD65D69E}"/>
-    <hyperlink ref="F26" r:id="rId7" xr:uid="{BC2E73A6-CC84-4897-A562-432D2F10BD7D}"/>
-    <hyperlink ref="F25" r:id="rId8" xr:uid="{C011FDAA-A7A1-4B75-A45E-5CDE4F833888}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{D4ED1D55-E4AC-4C6B-85A0-E974BD65D69E}"/>
+    <hyperlink ref="F27" r:id="rId7" xr:uid="{BC2E73A6-CC84-4897-A562-432D2F10BD7D}"/>
+    <hyperlink ref="F26" r:id="rId8" xr:uid="{C011FDAA-A7A1-4B75-A45E-5CDE4F833888}"/>
     <hyperlink ref="F13" r:id="rId9" xr:uid="{42144703-9840-4D52-B6CF-A348CB56A38A}"/>
-    <hyperlink ref="F14" r:id="rId10" xr:uid="{ADDDCEE4-578C-45E1-9160-50C0D7BE79D1}"/>
-    <hyperlink ref="F15" r:id="rId11" xr:uid="{529BAA51-BE48-4995-9085-384F5A2A592D}"/>
-    <hyperlink ref="F17" r:id="rId12" xr:uid="{343CB611-B772-4C93-AFF7-0CD5DFC56855}"/>
-    <hyperlink ref="F18" r:id="rId13" xr:uid="{F7A28780-F589-4302-9A4A-DD5CCF7C2BBB}"/>
+    <hyperlink ref="F15" r:id="rId10" xr:uid="{ADDDCEE4-578C-45E1-9160-50C0D7BE79D1}"/>
+    <hyperlink ref="F16" r:id="rId11" xr:uid="{529BAA51-BE48-4995-9085-384F5A2A592D}"/>
+    <hyperlink ref="F18" r:id="rId12" xr:uid="{343CB611-B772-4C93-AFF7-0CD5DFC56855}"/>
+    <hyperlink ref="F19" r:id="rId13" xr:uid="{F7A28780-F589-4302-9A4A-DD5CCF7C2BBB}"/>
     <hyperlink ref="F7" r:id="rId14" xr:uid="{7ED2F2C6-A380-4AEA-A739-C47C168E02C1}"/>
-    <hyperlink ref="F19" r:id="rId15" xr:uid="{D1212EC4-0F69-4B44-9722-85C729924D3D}"/>
-    <hyperlink ref="F20" r:id="rId16" xr:uid="{66DFDC9B-438A-4867-8871-0589DC4464E2}"/>
-    <hyperlink ref="F23" r:id="rId17" xr:uid="{8FC23CCB-8E9D-4FB2-978B-302E91115EF9}"/>
+    <hyperlink ref="F20" r:id="rId15" xr:uid="{D1212EC4-0F69-4B44-9722-85C729924D3D}"/>
+    <hyperlink ref="F21" r:id="rId16" xr:uid="{66DFDC9B-438A-4867-8871-0589DC4464E2}"/>
+    <hyperlink ref="F24" r:id="rId17" xr:uid="{8FC23CCB-8E9D-4FB2-978B-302E91115EF9}"/>
+    <hyperlink ref="F2" r:id="rId18" xr:uid="{FB7223F2-3337-4A54-9C9F-F133E0E5A8B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>